<commit_message>
Added tests and input validation
</commit_message>
<xml_diff>
--- a/test_data/course_grades.xlsx
+++ b/test_data/course_grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Student number</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>RoundedGrade</t>
+  </si>
+  <si>
+    <t>Empty</t>
   </si>
 </sst>
 </file>
@@ -113,8 +116,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D8" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Student number"/>
     <tableColumn id="3" name="Name"/>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,75 +446,83 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>45678</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <f>ROUND(4.2,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>56789</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <f>ROUND(4.9, 0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>23456</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D5" s="1">
         <f>ROUND(2.2, 0)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>34567</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D6" s="1">
         <f>ROUND(3.2,0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>45678</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <f>ROUND(4.2,0)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>56789</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
-        <f>ROUND(4.9, 0)</f>
-        <v>5</v>
-      </c>
-    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>99999</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>67890</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>